<commit_message>
Added Intro, Summary & Visualization
</commit_message>
<xml_diff>
--- a/GDP.xlsx
+++ b/GDP.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18120"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Country</t>
   </si>
@@ -563,13 +563,16 @@
   </si>
   <si>
     <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>NLGDP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,21 +909,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C181"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,8 +933,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -941,8 +947,12 @@
       <c r="C2" s="1">
         <v>42.84</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <f>(LN(B2))</f>
+        <v>6.2146080984221914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -952,8 +962,12 @@
       <c r="C3" s="1">
         <v>47.34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">(LN(B3))</f>
+        <v>6.2146080984221914</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -963,8 +977,12 @@
       <c r="C4" s="1">
         <v>44.56</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6.3969296552161463</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -974,8 +992,12 @@
       <c r="C5" s="1">
         <v>43.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>6.3969296552161463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -985,8 +1007,12 @@
       <c r="C6" s="1">
         <v>71.400000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>6.3969296552161463</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -996,8 +1022,12 @@
       <c r="C7" s="1">
         <v>37.979999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>6.3969296552161463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1007,8 +1037,12 @@
       <c r="C8" s="1">
         <v>50.02</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6.5510803350434044</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1018,8 +1052,12 @@
       <c r="C9" s="1">
         <v>48.93</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6.5510803350434044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1029,8 +1067,12 @@
       <c r="C10" s="1">
         <v>41.24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>6.5510803350434044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1040,8 +1082,12 @@
       <c r="C11" s="1">
         <v>46.97</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1051,8 +1097,12 @@
       <c r="C12" s="1">
         <v>42.21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1062,8 +1112,12 @@
       <c r="C13" s="1">
         <v>46.97</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1073,8 +1127,12 @@
       <c r="C14" s="1">
         <v>56.14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1084,8 +1142,12 @@
       <c r="C15" s="1">
         <v>60.97</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1095,8 +1157,12 @@
       <c r="C16" s="1">
         <v>35.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6.6846117276679271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1106,8 +1172,12 @@
       <c r="C17" s="1">
         <v>51.01</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>6.8023947633243109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1117,8 +1187,12 @@
       <c r="C18" s="1">
         <v>45.43</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>6.8023947633243109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1128,8 +1202,12 @@
       <c r="C19" s="1">
         <v>48.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6.9077552789821368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1139,8 +1217,12 @@
       <c r="C20" s="1">
         <v>45.22</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>6.9077552789821368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1150,8 +1232,12 @@
       <c r="C21" s="1">
         <v>64.37</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>6.9077552789821368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1161,8 +1247,12 @@
       <c r="C22" s="1">
         <v>44.46</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>7.0030654587864616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1172,8 +1262,12 @@
       <c r="C23" s="1">
         <v>72.680000000000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>7.0030654587864616</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1183,8 +1277,12 @@
       <c r="C24" s="1">
         <v>51.08</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>7.0030654587864616</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1194,8 +1292,12 @@
       <c r="C25" s="1">
         <v>41.71</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>7.0030654587864616</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1205,8 +1307,12 @@
       <c r="C26" s="1">
         <v>48.51</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>7.0900768357760917</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1216,8 +1322,12 @@
       <c r="C27" s="1">
         <v>31.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>7.0900768357760917</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1227,8 +1337,12 @@
       <c r="C28" s="1">
         <v>66.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>7.0900768357760917</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1238,8 +1352,12 @@
       <c r="C29" s="1">
         <v>39.33</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>7.1701195434496281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1249,8 +1367,12 @@
       <c r="C30" s="1">
         <v>70.790000000000006</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>7.1701195434496281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1260,8 +1382,12 @@
       <c r="C31" s="1">
         <v>42.65</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>7.2442275156033498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1271,8 +1397,12 @@
       <c r="C32" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>7.2442275156033498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1282,8 +1412,12 @@
       <c r="C33" s="1">
         <v>53.58</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>7.2442275156033498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1293,8 +1427,12 @@
       <c r="C34" s="1">
         <v>44.88</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>7.2442275156033498</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1304,8 +1442,12 @@
       <c r="C35" s="1">
         <v>53.43</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>7.3132203870903014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1315,8 +1457,12 @@
       <c r="C36" s="1">
         <v>67.81</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>7.3132203870903014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1326,8 +1472,12 @@
       <c r="C37" s="1">
         <v>63.66</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>7.3777589082278725</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1337,8 +1487,12 @@
       <c r="C38" s="1">
         <v>51.61</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>7.3777589082278725</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1348,8 +1502,12 @@
       <c r="C39" s="1">
         <v>56.37</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>7.3777589082278725</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1359,8 +1517,12 @@
       <c r="C40" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>7.4383835300443071</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1370,8 +1532,12 @@
       <c r="C41" s="1">
         <v>54.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>7.4383835300443071</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1381,8 +1547,12 @@
       <c r="C42" s="1">
         <v>54.38</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>7.4383835300443071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1392,8 +1562,12 @@
       <c r="C43" s="1">
         <v>48.05</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>7.4955419438842563</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1403,8 +1577,12 @@
       <c r="C44" s="1">
         <v>55.79</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>7.4955419438842563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1414,8 +1592,12 @@
       <c r="C45" s="1">
         <v>64.88</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>7.4955419438842563</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1425,8 +1607,12 @@
       <c r="C46" s="1">
         <v>51.93</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>7.4955419438842563</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1436,8 +1622,12 @@
       <c r="C47" s="1">
         <v>63.81</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>7.4955419438842563</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1447,8 +1637,12 @@
       <c r="C48" s="1">
         <v>61.33</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>7.5496091651545321</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1458,8 +1652,12 @@
       <c r="C49" s="1">
         <v>36.96</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>7.5496091651545321</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1469,8 +1667,12 @@
       <c r="C50" s="1">
         <v>57.92</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>7.5496091651545321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1480,8 +1682,12 @@
       <c r="C51" s="1">
         <v>57.73</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>7.5496091651545321</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1491,8 +1697,12 @@
       <c r="C52" s="1">
         <v>39.01</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>7.5496091651545321</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1502,8 +1712,12 @@
       <c r="C53" s="1">
         <v>49.54</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>7.6496926237115144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1513,8 +1727,12 @@
       <c r="C54" s="1">
         <v>62.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>7.6496926237115144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1524,8 +1742,12 @@
       <c r="C55" s="1">
         <v>64.19</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>7.696212639346407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1535,8 +1757,12 @@
       <c r="C56" s="1">
         <v>56.53</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>7.696212639346407</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1546,8 +1772,12 @@
       <c r="C57" s="1">
         <v>69.680000000000007</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>7.7406644019172415</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1557,8 +1787,12 @@
       <c r="C58" s="1">
         <v>64.78</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>7.7832240163360371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1568,8 +1802,12 @@
       <c r="C59" s="1">
         <v>64.760000000000005</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>7.8240460108562919</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1579,8 +1817,12 @@
       <c r="C60" s="1">
         <v>70.05</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>7.8240460108562919</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1590,8 +1832,12 @@
       <c r="C61" s="1">
         <v>66.650000000000006</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>7.8632667240095735</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1601,8 +1847,12 @@
       <c r="C62" s="1">
         <v>60.6</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>7.8632667240095735</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1612,8 +1862,12 @@
       <c r="C63" s="1">
         <v>63.62</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>7.9724660159745655</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1623,8 +1877,12 @@
       <c r="C64" s="1">
         <v>61.71</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>7.9724660159745655</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -1634,8 +1892,12 @@
       <c r="C65" s="1">
         <v>76.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>7.9724660159745655</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -1645,8 +1907,12 @@
       <c r="C66" s="1">
         <v>36.94</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>8.0063675676502459</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -1656,8 +1922,12 @@
       <c r="C67" s="1">
         <v>68.94</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="1">(LN(B67))</f>
+        <v>8.0709060887878188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -1667,8 +1937,12 @@
       <c r="C68" s="1">
         <v>71.89</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>8.1016777474545716</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -1678,8 +1952,12 @@
       <c r="C69" s="1">
         <v>69.39</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>8.1016777474545716</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -1689,8 +1967,12 @@
       <c r="C70" s="1">
         <v>63.16</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>8.1315307106042525</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -1700,8 +1982,12 @@
       <c r="C71" s="1">
         <v>66.680000000000007</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>8.1605182474775049</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -1711,8 +1997,12 @@
       <c r="C72" s="1">
         <v>72.62</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>8.2160880986323157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -1722,8 +2012,12 @@
       <c r="C73" s="1">
         <v>75.849999999999994</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>8.2687318321177372</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -1733,8 +2027,12 @@
       <c r="C74" s="1">
         <v>70.040000000000006</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>8.2940496401020276</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -1744,8 +2042,12 @@
       <c r="C75" s="1">
         <v>69.23</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>8.2940496401020276</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -1755,8 +2057,12 @@
       <c r="C76" s="1">
         <v>70.41</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>8.2940496401020276</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -1766,8 +2072,12 @@
       <c r="C77" s="1">
         <v>63.09</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>8.2940496401020276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -1777,8 +2087,12 @@
       <c r="C78" s="1">
         <v>65.23</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>8.3187422526923989</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -1788,8 +2102,12 @@
       <c r="C79" s="1">
         <v>77.88</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>8.3663703016816537</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -1799,8 +2117,12 @@
       <c r="C80" s="1">
         <v>72.37</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>8.4118326757584114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -1810,8 +2132,12 @@
       <c r="C81" s="1">
         <v>69.290000000000006</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>8.4338115824771869</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -1821,8 +2147,12 @@
       <c r="C82" s="1">
         <v>74.400000000000006</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>8.4553177876981493</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -1832,8 +2162,12 @@
       <c r="C83" s="1">
         <v>72.069999999999993</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>8.4763711968959825</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -1843,8 +2177,12 @@
       <c r="C84" s="1">
         <v>70.62</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>8.4763711968959825</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -1854,8 +2192,12 @@
       <c r="C85" s="1">
         <v>73.81</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>8.4763711968959825</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -1865,8 +2207,12 @@
       <c r="C86" s="1">
         <v>39.47</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>8.4969904840987187</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -1876,8 +2222,12 @@
       <c r="C87" s="1">
         <v>72.22</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>8.5171931914162382</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -1887,8 +2237,12 @@
       <c r="C88" s="1">
         <v>70.88</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>8.536995818712418</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -1898,8 +2252,12 @@
       <c r="C89" s="1">
         <v>66.5</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>8.5941542325523663</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -1909,8 +2267,12 @@
       <c r="C90" s="1">
         <v>57.12</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>8.6125033712205621</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -1920,8 +2282,12 @@
       <c r="C91" s="1">
         <v>74.12</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>8.6125033712205621</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -1931,8 +2297,12 @@
       <c r="C92" s="1">
         <v>68.88</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>8.66561319653451</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -1942,8 +2312,12 @@
       <c r="C93" s="1">
         <v>61.19</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>8.66561319653451</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -1953,8 +2327,12 @@
       <c r="C94" s="1">
         <v>67.959999999999994</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>8.6995147482101913</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -1964,8 +2342,12 @@
       <c r="C95" s="1">
         <v>70.540000000000006</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>8.6995147482101913</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -1975,8 +2357,12 @@
       <c r="C96" s="1">
         <v>72.290000000000006</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>8.7160440501614023</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -1986,8 +2372,12 @@
       <c r="C97" s="1">
         <v>68.430000000000007</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>8.7160440501614023</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>99</v>
       </c>
@@ -1997,8 +2387,12 @@
       <c r="C98" s="1">
         <v>71.14</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>8.7483049123796235</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2008,8 +2402,12 @@
       <c r="C99" s="1">
         <v>72.319999999999993</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>8.7483049123796235</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -2019,8 +2417,12 @@
       <c r="C100" s="1">
         <v>63.48</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>8.7483049123796235</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -2030,8 +2432,12 @@
       <c r="C101" s="1">
         <v>76.069999999999993</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>8.7640532693477624</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -2041,8 +2447,12 @@
       <c r="C102" s="1">
         <v>74.489999999999995</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>8.8098628053790566</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -2052,8 +2462,12 @@
       <c r="C103" s="1">
         <v>71.8</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>8.8098628053790566</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -2063,8 +2477,12 @@
       <c r="C104" s="1">
         <v>74.400000000000006</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>8.8392766905853506</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -2074,8 +2492,12 @@
       <c r="C105" s="1">
         <v>70.62</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>8.8536654280374503</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -2085,8 +2507,12 @@
       <c r="C106" s="1">
         <v>69.349999999999994</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>8.8536654280374503</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>108</v>
       </c>
@@ -2096,8 +2522,12 @@
       <c r="C107" s="1">
         <v>42.77</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>8.8818363050041462</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -2107,8 +2537,12 @@
       <c r="C108" s="1">
         <v>71.239999999999995</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>8.9092352791922611</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -2118,8 +2552,12 @@
       <c r="C109" s="1">
         <v>71.13</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>8.9359035262744229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -2129,8 +2567,12 @@
       <c r="C110" s="1">
         <v>71.8</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>8.9359035262744229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>112</v>
       </c>
@@ -2140,8 +2582,12 @@
       <c r="C111" s="1">
         <v>77.53</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>8.9746180384551124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -2151,8 +2597,12 @@
       <c r="C112" s="1">
         <v>76.69</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>9.0240107937846901</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>114</v>
       </c>
@@ -2162,8 +2612,12 @@
       <c r="C113" s="1">
         <v>67.66</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>9.0938065557202314</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -2173,8 +2627,12 @@
       <c r="C114" s="1">
         <v>32.26</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>9.1049798563183568</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>116</v>
       </c>
@@ -2184,8 +2642,12 @@
       <c r="C115" s="1">
         <v>72.3</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>9.1049798563183568</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -2195,8 +2657,12 @@
       <c r="C116" s="1">
         <v>71.67</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>9.1049798563183568</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -2206,8 +2672,12 @@
       <c r="C117" s="1">
         <v>76.430000000000007</v>
       </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>9.1160296925049416</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>119</v>
       </c>
@@ -2217,8 +2687,12 @@
       <c r="C118" s="1">
         <v>69.59</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>9.1590470775886317</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -2228,8 +2702,12 @@
       <c r="C119" s="1">
         <v>76.349999999999994</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>9.2002900361226807</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -2239,8 +2717,12 @@
       <c r="C120" s="1">
         <v>69.31</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>9.2301429992723616</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>122</v>
       </c>
@@ -2250,8 +2732,12 @@
       <c r="C121" s="1">
         <v>74.37</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>9.2686092801001578</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>123</v>
       </c>
@@ -2261,8 +2747,12 @@
       <c r="C122" s="1">
         <v>46.56</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>9.2779990204499967</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -2272,8 +2762,12 @@
       <c r="C123" s="1">
         <v>73.91</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>9.3147003873004248</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>125</v>
       </c>
@@ -2283,8 +2777,12 @@
       <c r="C124" s="1">
         <v>75.48</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>9.3236690572831851</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>126</v>
       </c>
@@ -2294,8 +2792,12 @@
       <c r="C125" s="1">
         <v>75.38</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="D125">
+        <f t="shared" si="1"/>
+        <v>9.3413686343825866</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>127</v>
       </c>
@@ -2305,8 +2807,12 @@
       <c r="C126" s="1">
         <v>71.8</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="D126">
+        <f t="shared" si="1"/>
+        <v>9.3413686343825866</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>128</v>
       </c>
@@ -2316,8 +2822,12 @@
       <c r="C127" s="1">
         <v>69.599999999999994</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="D127">
+        <f t="shared" si="1"/>
+        <v>9.3413686343825866</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>129</v>
       </c>
@@ -2327,8 +2837,12 @@
       <c r="C128" s="1">
         <v>68.73</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128">
+        <f t="shared" si="1"/>
+        <v>9.375854810453756</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>130</v>
       </c>
@@ -2338,8 +2852,12 @@
       <c r="C129" s="1">
         <v>70.31</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129">
+        <f t="shared" si="1"/>
+        <v>9.417354541360508</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -2349,8 +2867,12 @@
       <c r="C130" s="1">
         <v>75.87</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="D130">
+        <f t="shared" si="1"/>
+        <v>9.4572004499077078</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>132</v>
       </c>
@@ -2360,8 +2882,12 @@
       <c r="C131" s="1">
         <v>72.58</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="D131">
+        <f t="shared" ref="D131:D181" si="2">(LN(B131))</f>
+        <v>9.480367509189243</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>133</v>
       </c>
@@ -2371,8 +2897,12 @@
       <c r="C132" s="1">
         <v>74.430000000000007</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="D132">
+        <f t="shared" si="2"/>
+        <v>9.4955193142098455</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>134</v>
       </c>
@@ -2382,8 +2912,12 @@
       <c r="C133" s="1">
         <v>72.17</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133">
+        <f t="shared" si="2"/>
+        <v>9.5396441191187833</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>135</v>
       </c>
@@ -2393,8 +2927,12 @@
       <c r="C134" s="1">
         <v>78.72</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134">
+        <f t="shared" si="2"/>
+        <v>9.5749834855640916</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>136</v>
       </c>
@@ -2404,8 +2942,12 @@
       <c r="C135" s="1">
         <v>73.52</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="D135">
+        <f t="shared" si="2"/>
+        <v>9.6158054800843473</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>137</v>
       </c>
@@ -2415,8 +2957,12 @@
       <c r="C136" s="1">
         <v>75.180000000000007</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="D136">
+        <f t="shared" si="2"/>
+        <v>9.6614159913363995</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -2426,8 +2972,12 @@
       <c r="C137" s="1">
         <v>71.84</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="D137">
+        <f t="shared" si="2"/>
+        <v>9.6614159913363995</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -2437,8 +2987,12 @@
       <c r="C138" s="1">
         <v>65.709999999999994</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="D138">
+        <f t="shared" si="2"/>
+        <v>9.7231639984048464</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>140</v>
       </c>
@@ -2448,8 +3002,12 @@
       <c r="C139" s="1">
         <v>77.260000000000005</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="D139">
+        <f t="shared" si="2"/>
+        <v>9.7291341653913506</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -2459,8 +3017,12 @@
       <c r="C140" s="1">
         <v>73.72</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="D140">
+        <f t="shared" si="2"/>
+        <v>9.7350689009111644</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>142</v>
       </c>
@@ -2470,8 +3032,12 @@
       <c r="C141" s="1">
         <v>75.45</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="D141">
+        <f t="shared" si="2"/>
+        <v>9.7699561599116063</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>143</v>
       </c>
@@ -2481,8 +3047,12 @@
       <c r="C142" s="1">
         <v>78.430000000000007</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142">
+        <f t="shared" si="2"/>
+        <v>9.7813199185619197</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>144</v>
       </c>
@@ -2492,8 +3062,12 @@
       <c r="C143" s="1">
         <v>75.36</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="D143">
+        <f t="shared" si="2"/>
+        <v>9.7869537362801768</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>145</v>
       </c>
@@ -2503,8 +3077,12 @@
       <c r="C144" s="1">
         <v>76.349999999999994</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="D144">
+        <f t="shared" si="2"/>
+        <v>9.7981270368783022</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -2514,8 +3092,12 @@
       <c r="C145" s="1">
         <v>76.650000000000006</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="D145">
+        <f t="shared" si="2"/>
+        <v>9.8521942581485771</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>147</v>
       </c>
@@ -2525,8 +3107,12 @@
       <c r="C146" s="1">
         <v>75.510000000000005</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="D146">
+        <f t="shared" si="2"/>
+        <v>9.8521942581485771</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>148</v>
       </c>
@@ -2536,8 +3122,12 @@
       <c r="C147" s="1">
         <v>81.87</v>
       </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="D147">
+        <f t="shared" si="2"/>
+        <v>9.87302834505142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -2547,8 +3137,12 @@
       <c r="C148" s="1">
         <v>79.02</v>
       </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="D148">
+        <f t="shared" si="2"/>
+        <v>9.8934372166826261</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -2558,8 +3152,12 @@
       <c r="C149" s="1">
         <v>78.89</v>
       </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="D149">
+        <f t="shared" si="2"/>
+        <v>9.9034875525361272</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>151</v>
       </c>
@@ -2569,8 +3167,12 @@
       <c r="C150" s="1">
         <v>73.14</v>
       </c>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="D150">
+        <f t="shared" si="2"/>
+        <v>9.9758082141157534</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>152</v>
       </c>
@@ -2580,8 +3182,12 @@
       <c r="C151" s="1">
         <v>78.319999999999993</v>
       </c>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="D151">
+        <f t="shared" si="2"/>
+        <v>9.9804485936722571</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>153</v>
       </c>
@@ -2591,8 +3197,12 @@
       <c r="C152" s="1">
         <v>79.23</v>
       </c>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="D152">
+        <f t="shared" si="2"/>
+        <v>9.9987977323404529</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -2602,8 +3212,12 @@
       <c r="C153" s="1">
         <v>74.75</v>
       </c>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="D153">
+        <f t="shared" si="2"/>
+        <v>10.051907557654401</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -2613,8 +3227,12 @@
       <c r="C154" s="1">
         <v>76.87</v>
       </c>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="D154">
+        <f t="shared" si="2"/>
+        <v>10.060491301345794</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -2624,8 +3242,12 @@
       <c r="C155" s="1">
         <v>74.3</v>
       </c>
-    </row>
-    <row r="156" spans="1:3">
+      <c r="D155">
+        <f t="shared" si="2"/>
+        <v>10.069001991013701</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -2635,8 +3257,12 @@
       <c r="C156" s="1">
         <v>80.42</v>
       </c>
-    </row>
-    <row r="157" spans="1:3">
+      <c r="D156">
+        <f t="shared" si="2"/>
+        <v>10.073230327123223</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -2646,8 +3272,12 @@
       <c r="C157" s="1">
         <v>79.400000000000006</v>
       </c>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="D157">
+        <f t="shared" si="2"/>
+        <v>10.192418844388341</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -2657,8 +3287,12 @@
       <c r="C158" s="1">
         <v>83.49</v>
       </c>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="D158">
+        <f t="shared" si="2"/>
+        <v>10.196157166498947</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -2668,8 +3302,12 @@
       <c r="C159" s="1">
         <v>79.97</v>
       </c>
-    </row>
-    <row r="160" spans="1:3">
+      <c r="D159">
+        <f t="shared" si="2"/>
+        <v>10.196157166498947</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -2679,8 +3317,12 @@
       <c r="C160" s="1">
         <v>77.92</v>
       </c>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="D160">
+        <f t="shared" si="2"/>
+        <v>10.218298292376161</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -2690,8 +3332,12 @@
       <c r="C161" s="1">
         <v>79.28</v>
       </c>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="D161">
+        <f t="shared" si="2"/>
+        <v>10.225571051705241</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -2701,8 +3347,12 @@
       <c r="C162" s="1">
         <v>78.42</v>
       </c>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="D162">
+        <f t="shared" si="2"/>
+        <v>10.225571051705241</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -2712,8 +3362,12 @@
       <c r="C163" s="1">
         <v>78.16</v>
       </c>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="D163">
+        <f t="shared" si="2"/>
+        <v>10.229187692175429</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -2723,8 +3377,12 @@
       <c r="C164" s="1">
         <v>80.930000000000007</v>
       </c>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="D164">
+        <f t="shared" si="2"/>
+        <v>10.247077256926206</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -2734,8 +3392,12 @@
       <c r="C165" s="1">
         <v>77.98</v>
       </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="D165">
+        <f t="shared" si="2"/>
+        <v>10.257659366256743</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -2745,8 +3407,12 @@
       <c r="C166" s="1">
         <v>78.739999999999995</v>
       </c>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="D166">
+        <f t="shared" si="2"/>
+        <v>10.261161996807944</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -2756,8 +3422,12 @@
       <c r="C167" s="1">
         <v>79.930000000000007</v>
       </c>
-    </row>
-    <row r="168" spans="1:3">
+      <c r="D167">
+        <f t="shared" si="2"/>
+        <v>10.268130666124037</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -2767,8 +3437,12 @@
       <c r="C168" s="1">
         <v>80.13</v>
       </c>
-    </row>
-    <row r="169" spans="1:3">
+      <c r="D168">
+        <f t="shared" si="2"/>
+        <v>10.275051108968611</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -2778,8 +3452,12 @@
       <c r="C169" s="1">
         <v>78.290000000000006</v>
       </c>
-    </row>
-    <row r="170" spans="1:3">
+      <c r="D169">
+        <f t="shared" si="2"/>
+        <v>10.278493453159584</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -2789,8 +3467,12 @@
       <c r="C170" s="1">
         <v>77.349999999999994</v>
       </c>
-    </row>
-    <row r="171" spans="1:3">
+      <c r="D170">
+        <f t="shared" si="2"/>
+        <v>10.295529640312152</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -2800,8 +3482,12 @@
       <c r="C171" s="1">
         <v>79.83</v>
       </c>
-    </row>
-    <row r="172" spans="1:3">
+      <c r="D171">
+        <f t="shared" si="2"/>
+        <v>10.302263672493496</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -2811,8 +3497,12 @@
       <c r="C172" s="1">
         <v>78.17</v>
       </c>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="D172">
+        <f t="shared" si="2"/>
+        <v>10.308952660644293</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -2822,8 +3512,12 @@
       <c r="C173" s="1">
         <v>79.8</v>
       </c>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="D173">
+        <f t="shared" si="2"/>
+        <v>10.338511462885837</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -2833,8 +3527,12 @@
       <c r="C174" s="1">
         <v>77.099999999999994</v>
       </c>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="D174">
+        <f t="shared" si="2"/>
+        <v>10.344963098167325</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -2844,8 +3542,12 @@
       <c r="C175" s="1">
         <v>79.989999999999995</v>
       </c>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="D175">
+        <f t="shared" si="2"/>
+        <v>10.395130356885344</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -2855,8 +3557,12 @@
       <c r="C176" s="1">
         <v>77.41</v>
       </c>
-    </row>
-    <row r="177" spans="1:3">
+      <c r="D176">
+        <f t="shared" si="2"/>
+        <v>10.491274217438248</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -2866,8 +3572,12 @@
       <c r="C177" s="1">
         <v>79.09</v>
       </c>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="D177">
+        <f t="shared" si="2"/>
+        <v>10.54006438160768</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -2877,8 +3587,12 @@
       <c r="C178" s="1">
         <v>77.14</v>
       </c>
-    </row>
-    <row r="179" spans="1:3">
+      <c r="D178">
+        <f t="shared" si="2"/>
+        <v>10.54006438160768</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -2888,8 +3602,12 @@
       <c r="C179" s="1">
         <v>78.930000000000007</v>
       </c>
-    </row>
-    <row r="180" spans="1:3">
+      <c r="D179">
+        <f t="shared" si="2"/>
+        <v>10.596634733096073</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -2899,8 +3617,12 @@
       <c r="C180" s="1">
         <v>80.040000000000006</v>
       </c>
-    </row>
-    <row r="181" spans="1:3">
+      <c r="D180">
+        <f t="shared" si="2"/>
+        <v>10.596634733096073</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -2909,6 +3631,10 @@
       </c>
       <c r="C181" s="1">
         <v>77.66</v>
+      </c>
+      <c r="D181">
+        <f t="shared" si="2"/>
+        <v>10.916904995141007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>